<commit_message>
added ability to highlight previous answer
</commit_message>
<xml_diff>
--- a/extras/example_form/Sample Form - Display Roster in Table.xlsx
+++ b/extras/example_form/Sample Form - Display Roster in Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\GitHub\table-list\extras\example_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E581B24C-8824-4292-802C-D2F0585F99D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C211D2-BA67-452E-867A-EE079C98208A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="429">
   <si>
     <t>type</t>
   </si>
@@ -4743,9 +4743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
+      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.6"/>
@@ -6146,9 +6146,7 @@
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
       <c r="H40" s="17"/>
-      <c r="I40" s="14" t="s">
-        <v>79</v>
-      </c>
+      <c r="I40" s="14"/>
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
       <c r="L40" s="14"/>
@@ -33519,7 +33517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
@@ -61684,7 +61682,7 @@
       </c>
       <c r="C2" s="11" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2005081251</v>
+        <v>2005082031</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="18"/>
@@ -61951,7 +61949,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="202.8" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:30" ht="187.2" x14ac:dyDescent="0.6">
       <c r="A6" s="23" t="s">
         <v>67</v>
       </c>
@@ -62413,7 +62411,7 @@
       <c r="AC16" s="26"/>
       <c r="AD16" s="26"/>
     </row>
-    <row r="17" spans="1:30" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:30" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A17" s="26" t="s">
         <v>135</v>
       </c>
@@ -68959,7 +68957,7 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="312" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:26" ht="296.39999999999998" x14ac:dyDescent="0.6">
       <c r="A6" s="23" t="s">
         <v>408</v>
       </c>

</xml_diff>